<commit_message>
Slide Judul & Menambahkan Logbook+Burndown Chart Kedua
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6365D8B-ACB8-406D-B924-EC20D7D816D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B4F0AE-537D-4BFD-B55B-74DC18FA7143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8D8DF68-8B82-4C3F-A7EB-E4324A6E059A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8D8DF68-8B82-4C3F-A7EB-E4324A6E059A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +48,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
   <si>
     <t>Waktu sebenarnya</t>
@@ -613,6 +617,9 @@
                 <c:pt idx="1">
                   <c:v>12</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1723,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84766C9A-066C-40D2-9700-57023201DC25}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1741,7 +1748,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
       <c r="B2" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -1767,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
@@ -1781,16 +1788,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -1799,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -1807,16 +1814,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2">
         <v>4</v>
@@ -1825,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -1833,16 +1840,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2">
         <v>4</v>
@@ -1851,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -1859,16 +1866,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2">
         <v>4</v>
@@ -1881,16 +1888,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2">
         <v>4</v>
@@ -1903,16 +1910,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2">
         <v>4</v>
@@ -1925,16 +1932,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="7">
         <v>4</v>
@@ -1947,16 +1954,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" s="7">
         <v>4</v>
@@ -1969,16 +1976,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="7">
         <v>4</v>
@@ -1991,16 +1998,16 @@
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F14" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="2">
         <v>4</v>
@@ -2013,16 +2020,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2">
         <v>4</v>
@@ -2035,16 +2042,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" s="2">
         <v>4</v>
@@ -2057,16 +2064,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2">
         <v>4</v>
@@ -2079,16 +2086,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="G18" s="2">
         <v>8</v>
@@ -2101,16 +2108,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
@@ -2131,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2956EE38-F0D5-4F33-925A-15CFCAC533DA}">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2143,27 +2150,27 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -2171,13 +2178,15 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -2185,13 +2194,15 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -2199,13 +2210,15 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2213,13 +2226,15 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2227,13 +2242,15 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -2241,13 +2258,15 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2255,13 +2274,15 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2269,13 +2290,15 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -2283,27 +2306,29 @@
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="13" spans="2:7">
       <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f>SUM(C3:C11)</f>
@@ -2313,12 +2338,15 @@
         <f>C14-(SUM(D3:D11))</f>
         <v>12</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <f>D14-(SUM(E3:E11))</f>
+        <v>6</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2">
         <f>SUM(C3:C11)</f>
@@ -2341,4 +2369,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CEBF59-E0E2-41E0-B576-C99A52E8A048}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C39" sqref="C38:C39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Logbook dan Burndown Chart Ketiga
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\Tugas\TKPPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B4F0AE-537D-4BFD-B55B-74DC18FA7143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B3AA0F-7FAB-4D79-8025-0565B4AF760E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8D8DF68-8B82-4C3F-A7EB-E4324A6E059A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Waktu sebenarnya</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Hari 0</t>
   </si>
   <si>
-    <t>Menambahkan animasi ketika slide judul berganti</t>
-  </si>
-  <si>
     <t>Presenter</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>Membuat definisi arti dari Sistem BUS</t>
   </si>
   <si>
-    <t>Menambahkan animasi ketika slide definisi bus berganti</t>
-  </si>
-  <si>
     <t>memperlihatkan pengertian lanjut tentang control BUS yang merupakan bagian dari BUS</t>
   </si>
   <si>
@@ -203,9 +194,6 @@
     <t>Menambahkan gambar struktur BUS</t>
   </si>
   <si>
-    <t>Menambahkan animasi ketika slide interkoneksi bus berganti</t>
-  </si>
-  <si>
     <t>Topik : BUS</t>
   </si>
   <si>
@@ -213,6 +201,24 @@
   </si>
   <si>
     <t>penonton dapat memahami bahwa persentasi telah berakhir</t>
+  </si>
+  <si>
+    <t>Mendesign tulisan dan slide judul</t>
+  </si>
+  <si>
+    <t>Mendesign tulisan dan slide definisi BUS</t>
+  </si>
+  <si>
+    <t>Mendesign tulisan dan slide interkoneksi BUS</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>memperlihatkan animasi pada setiap perubahan slide dari BUS</t>
+  </si>
+  <si>
+    <t>penonton dapat lebih terkesan dengan slide yang dibawakan presenter</t>
   </si>
 </sst>
 </file>
@@ -238,14 +244,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -283,6 +281,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -299,13 +305,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -346,8 +352,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -359,9 +365,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,25 +379,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -619,6 +625,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1728,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84766C9A-066C-40D2-9700-57023201DC25}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1747,15 +1756,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="B2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -1774,7 +1783,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
@@ -1788,16 +1797,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>37</v>
+      <c r="F5" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -1805,8 +1814,8 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
+      <c r="I5" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -1814,16 +1823,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G6" s="2">
         <v>4</v>
@@ -1831,8 +1840,8 @@
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>7</v>
+      <c r="I6" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -1840,16 +1849,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G7" s="2">
         <v>4</v>
@@ -1857,8 +1866,8 @@
       <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
+      <c r="I7" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -1866,16 +1875,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G8" s="2">
         <v>4</v>
@@ -1888,16 +1897,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G9" s="2">
         <v>4</v>
@@ -1910,16 +1919,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G10" s="2">
         <v>4</v>
@@ -1928,86 +1937,86 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="7">
+        <v>48</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="6">
         <v>4</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="7">
+        <v>49</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="6">
         <v>4</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="7">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="6">
         <v>4</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="2">
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="G14" s="2">
         <v>4</v>
@@ -2016,20 +2025,20 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G15" s="2">
         <v>4</v>
@@ -2042,16 +2051,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G16" s="2">
         <v>4</v>
@@ -2060,20 +2069,20 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G17" s="2">
         <v>4</v>
@@ -2086,16 +2095,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>43</v>
+      <c r="F18" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="G18" s="2">
         <v>8</v>
@@ -2108,22 +2117,44 @@
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>43</v>
+        <v>57</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="6">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2139,7 +2170,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2149,28 +2180,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>9</v>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -2181,12 +2212,16 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -2197,12 +2232,16 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -2213,12 +2252,16 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2229,12 +2272,16 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2245,12 +2292,16 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -2261,12 +2312,16 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2277,12 +2332,16 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2293,12 +2352,16 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -2309,26 +2372,30 @@
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="5" t="s">
-        <v>8</v>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <f>SUM(C3:C11)</f>
@@ -2342,11 +2409,14 @@
         <f>D14-(SUM(E3:E11))</f>
         <v>6</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <f>E14-(SUM(F3:F11))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="5" t="s">
-        <v>11</v>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <f>SUM(C3:C11)</f>

</xml_diff>

<commit_message>
edit logbook dan excel tgl 23
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\Tugas\TKPPL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B3AA0F-7FAB-4D79-8025-0565B4AF760E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8D8DF68-8B82-4C3F-A7EB-E4324A6E059A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -219,13 +214,34 @@
   </si>
   <si>
     <t>penonton dapat lebih terkesan dengan slide yang dibawakan presenter</t>
+  </si>
+  <si>
+    <t>Membuat kelemahan pada BUS</t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>Membuat slide prinsip operasi BUS</t>
+  </si>
+  <si>
+    <t>Membuat faktor-faktor kelemahan pada BUS</t>
+  </si>
+  <si>
+    <t>Membuat slide arsitektur BUS</t>
+  </si>
+  <si>
+    <t>Menambahkan gambar arsitektur BUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,8 +305,16 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +336,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -355,7 +385,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,12 +421,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
@@ -417,7 +449,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -456,6 +488,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -464,26 +497,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -559,7 +572,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -633,7 +646,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -647,12 +660,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="880200048"/>
-        <c:axId val="880178416"/>
+        <c:axId val="203036160"/>
+        <c:axId val="203037696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="880200048"/>
+        <c:axId val="203036160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="880178416"/>
+        <c:crossAx val="203037696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,7 +717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="880178416"/>
+        <c:axId val="203037696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="880200048"/>
+        <c:crossAx val="203036160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -768,6 +782,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -799,14 +814,406 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Burndown Chart Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Waktu perkiraan (baseline)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$C$36:$F$36</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$C$37:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waktu sebenarnya</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$C$36:$F$36</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$C$38:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="137769728"/>
+        <c:axId val="137771264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="137769728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="137771264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="137771264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="137769728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1417,7 +1824,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1432,6 +1839,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1729,14 +2174,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84766C9A-066C-40D2-9700-57023201DC25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1756,15 +2201,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -1814,7 +2259,7 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1840,7 +2285,7 @@
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1866,7 +2311,7 @@
       <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2166,11 +2611,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2956EE38-F0D5-4F33-925A-15CFCAC533DA}">
-  <dimension ref="B2:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2179,7 +2636,12 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="1" spans="1:7" s="16" customFormat="1">
+      <c r="A1" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2199,7 +2661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="1:7">
       <c r="B3" s="3" t="s">
         <v>43</v>
       </c>
@@ -2219,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="1:7">
       <c r="B4" s="3" t="s">
         <v>44</v>
       </c>
@@ -2239,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="1:7">
       <c r="B5" s="3" t="s">
         <v>58</v>
       </c>
@@ -2259,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="1:7">
       <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
@@ -2279,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="1:7">
       <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
@@ -2299,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="1:7">
       <c r="B8" s="3" t="s">
         <v>59</v>
       </c>
@@ -2319,7 +2781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="1:7">
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
@@ -2339,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
         <v>54</v>
       </c>
@@ -2359,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="1:7">
       <c r="B11" s="3" t="s">
         <v>60</v>
       </c>
@@ -2379,7 +2841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="1:7">
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2393,7 +2855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="1:7">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -2414,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="1:7">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
@@ -2435,14 +2897,277 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:7" s="16" customFormat="1">
+      <c r="A23" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <f>SUM(D26:F26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="3"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" ref="G27:G34" si="0">SUM(D27:F27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="2">
+        <f>SUM(C26:C34)</f>
+        <v>6</v>
+      </c>
+      <c r="D37" s="2">
+        <f>C37-(SUM(D26:D34))</f>
+        <v>3</v>
+      </c>
+      <c r="E37" s="2">
+        <f>D37-(SUM(E26:E34))</f>
+        <v>3</v>
+      </c>
+      <c r="F37" s="2">
+        <f>E37-(SUM(F26:F34))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2">
+        <f>SUM(C26:C34)</f>
+        <v>6</v>
+      </c>
+      <c r="D38" s="2">
+        <f>C38-(C38/3)</f>
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
+        <f>D38-(C38/3)</f>
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <f>E38-(C38/3)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CEBF59-E0E2-41E0-B576-C99A52E8A048}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">

</xml_diff>

<commit_message>
Menambahkan slide yang menuliskan tentang pembagian arsitektur BUS
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -234,7 +234,22 @@
     <t>Membuat slide arsitektur BUS</t>
   </si>
   <si>
-    <t>Menambahkan gambar arsitektur BUS</t>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>Menambahkan gambar tradisional BUS</t>
+  </si>
+  <si>
+    <t>Menambahkan gambar high speed BUS</t>
+  </si>
+  <si>
+    <t>Membuat slide yang membagi jenis arsitektur BUS</t>
+  </si>
+  <si>
+    <t>Membuat slide penjelasan Traditional BUS</t>
+  </si>
+  <si>
+    <t>Membuat slide penjelasan High Speed BUS</t>
   </si>
 </sst>
 </file>
@@ -424,11 +439,11 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
@@ -662,11 +677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203036160"/>
-        <c:axId val="203037696"/>
+        <c:axId val="206329728"/>
+        <c:axId val="206331264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203036160"/>
+        <c:axId val="206329728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203037696"/>
+        <c:crossAx val="206331264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -717,7 +732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203037696"/>
+        <c:axId val="206331264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203036160"/>
+        <c:crossAx val="206329728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -957,16 +972,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,13 +1038,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>8.6666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4.3333333333333348</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1054,11 +1069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137769728"/>
-        <c:axId val="137771264"/>
+        <c:axId val="206370304"/>
+        <c:axId val="206371840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137769728"/>
+        <c:axId val="206370304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137771264"/>
+        <c:crossAx val="206371840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1109,7 +1124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137771264"/>
+        <c:axId val="206371840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1160,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137769728"/>
+        <c:crossAx val="206370304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1824,7 +1839,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1862,7 +1877,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2201,15 +2216,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -2624,10 +2639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2636,8 +2651,8 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" s="15" customFormat="1">
+      <c r="A1" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2897,8 +2912,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="16" customFormat="1">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:7" s="15" customFormat="1">
+      <c r="A23" s="14" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2944,12 +2959,14 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -2959,16 +2976,18 @@
       </c>
       <c r="G27" s="2">
         <f t="shared" ref="G27:G34" si="0">SUM(D27:F27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -2978,12 +2997,12 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -3004,7 +3023,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3024,9 +3043,11 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="B31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3038,16 +3059,16 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(D31:F31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -3059,16 +3080,16 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
+        <f>SUM(D32:F32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="B33" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3084,10 +3105,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="3"/>
+    <row r="34" spans="1:7">
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C34" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
@@ -3103,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="1:7">
       <c r="C36" s="4" t="s">
         <v>15</v>
       </c>
@@ -3117,46 +3140,51 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="1:7">
       <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="2">
         <f>SUM(C26:C34)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D37" s="2">
         <f>C37-(SUM(D26:D34))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E37" s="2">
         <f>D37-(SUM(E26:E34))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F37" s="2">
         <f>E37-(SUM(F26:F34))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="B38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="2">
         <f>SUM(C26:C34)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D38" s="2">
         <f>C38-(C38/3)</f>
-        <v>4</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="E38" s="2">
         <f>D38-(C38/3)</f>
-        <v>2</v>
+        <v>4.3333333333333348</v>
       </c>
       <c r="F38" s="2">
         <f>E38-(C38/3)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="15" customFormat="1">
+      <c r="A46" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mempercantik slide Arsitektur BUS
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Membuat slide penjelasan High Speed BUS</t>
+  </si>
+  <si>
+    <t>Mempercantik slide prinsip operasi BUS</t>
+  </si>
+  <si>
+    <t>Mempercantik slide kelemahan pada BUS</t>
+  </si>
+  <si>
+    <t>Mempercantik slide arsitektur BUS</t>
   </si>
 </sst>
 </file>
@@ -677,11 +686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206329728"/>
-        <c:axId val="206331264"/>
+        <c:axId val="182933376"/>
+        <c:axId val="182934912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206329728"/>
+        <c:axId val="182933376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,7 +733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206331264"/>
+        <c:crossAx val="182934912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -732,7 +741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206331264"/>
+        <c:axId val="182934912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206329728"/>
+        <c:crossAx val="182933376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -947,7 +956,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$36:$F$36</c:f>
+              <c:f>'Sprint 1'!$C$39:$F$39</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -967,21 +976,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$37:$F$37</c:f>
+              <c:f>'Sprint 1'!$C$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,7 +1022,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$36:$F$36</c:f>
+              <c:f>'Sprint 1'!$C$39:$F$39</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1033,18 +1042,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$38:$F$38</c:f>
+              <c:f>'Sprint 1'!$C$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6666666666666679</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3333333333333348</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1069,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206370304"/>
-        <c:axId val="206371840"/>
+        <c:axId val="182973952"/>
+        <c:axId val="182975488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206370304"/>
+        <c:axId val="182973952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206371840"/>
+        <c:crossAx val="182975488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206371840"/>
+        <c:axId val="182975488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1184,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206370304"/>
+        <c:crossAx val="182973952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,7 +1848,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1877,7 +1886,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2189,7 +2198,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2639,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2960,28 +2969,28 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ref="G27:G34" si="0">SUM(D27:F27)</f>
+        <f t="shared" ref="G27:G37" si="0">SUM(D27:F27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
@@ -3002,7 +3011,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -3023,16 +3032,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -3044,13 +3053,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -3059,19 +3068,19 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f>SUM(D31:F31)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
@@ -3080,37 +3089,37 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f>SUM(D32:F32)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
       </c>
       <c r="E33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
@@ -3126,59 +3135,122 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:7">
+      <c r="B35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="36" spans="1:7">
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="B37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="C39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="B37" s="4" t="s">
+    <row r="40" spans="1:7">
+      <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="2">
-        <f>SUM(C26:C34)</f>
-        <v>13</v>
-      </c>
-      <c r="D37" s="2">
-        <f>C37-(SUM(D26:D34))</f>
+      <c r="C40" s="2">
+        <f>SUM(C26:C37)</f>
+        <v>12</v>
+      </c>
+      <c r="D40" s="2">
+        <f>C40-(SUM(D26:D37))</f>
+        <v>7</v>
+      </c>
+      <c r="E40" s="2">
+        <f>D40-(SUM(E26:E37))</f>
+        <v>4</v>
+      </c>
+      <c r="F40" s="2">
+        <f>E40-(SUM(F26:F37))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="2">
+        <f>SUM(C26:C37)</f>
+        <v>12</v>
+      </c>
+      <c r="D41" s="2">
+        <f>C41-(C41/3)</f>
         <v>8</v>
       </c>
-      <c r="E37" s="2">
-        <f>D37-(SUM(E26:E34))</f>
-        <v>8</v>
-      </c>
-      <c r="F37" s="2">
-        <f>E37-(SUM(F26:F34))</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="B38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="2">
-        <f>SUM(C26:C34)</f>
-        <v>13</v>
-      </c>
-      <c r="D38" s="2">
-        <f>C38-(C38/3)</f>
-        <v>8.6666666666666679</v>
-      </c>
-      <c r="E38" s="2">
-        <f>D38-(C38/3)</f>
-        <v>4.3333333333333348</v>
-      </c>
-      <c r="F38" s="2">
-        <f>E38-(C38/3)</f>
+      <c r="E41" s="2">
+        <f>D41-(C41/3)</f>
+        <v>4</v>
+      </c>
+      <c r="F41" s="2">
+        <f>E41-(C41/3)</f>
         <v>0</v>
       </c>
     </row>
@@ -3186,6 +3258,20 @@
       <c r="A46" s="14" t="s">
         <v>70</v>
       </c>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
menambahkan gambar traditional bus dan high speed bus
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -686,11 +686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182933376"/>
-        <c:axId val="182934912"/>
+        <c:axId val="203184000"/>
+        <c:axId val="203185536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182933376"/>
+        <c:axId val="203184000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,7 +733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182934912"/>
+        <c:crossAx val="203185536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -741,7 +741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182934912"/>
+        <c:axId val="203185536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182933376"/>
+        <c:crossAx val="203184000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -990,7 +990,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1078,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182973952"/>
-        <c:axId val="182975488"/>
+        <c:axId val="203224576"/>
+        <c:axId val="203226112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182973952"/>
+        <c:axId val="203224576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182975488"/>
+        <c:crossAx val="203226112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1133,7 +1133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182975488"/>
+        <c:axId val="203226112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,7 +1184,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182973952"/>
+        <c:crossAx val="203224576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1848,7 +1848,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1886,7 +1886,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2198,7 +2198,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2650,8 +2650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3128,11 +3128,11 @@
         <v>0</v>
       </c>
       <c r="F34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3149,11 +3149,11 @@
         <v>0</v>
       </c>
       <c r="F35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3170,11 +3170,11 @@
         <v>0</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3191,11 +3191,11 @@
         <v>0</v>
       </c>
       <c r="F37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="F40" s="2">
         <f>E40-(SUM(F26:F37))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">

</xml_diff>

<commit_message>
Update logbook dan burndown chart Dec 26
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1463CB96-ED3E-4B9A-B2F5-5188463AA2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -259,13 +263,46 @@
   </si>
   <si>
     <t>Mempercantik slide arsitektur BUS</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>Mendesign Slide Control Bus</t>
+  </si>
+  <si>
+    <t>Membuat fungsi dari Control Bus</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Control Bus</t>
+  </si>
+  <si>
+    <t>Mendesign Slide Address Bus</t>
+  </si>
+  <si>
+    <t>Membuat fungsi dari Address Bus</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Addres Bus</t>
+  </si>
+  <si>
+    <t>Membuat Slide Data Bus</t>
+  </si>
+  <si>
+    <t>Membuat fungsi dari Data Bus</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Data Bus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +374,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +411,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -404,12 +454,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,13 +501,23 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,7 +534,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -512,7 +573,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -521,6 +581,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -533,7 +613,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$B$15</c:f>
+              <c:f>Sprint!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -556,7 +636,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$13:$F$13</c:f>
+              <c:f>Sprint!$C$14:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -576,7 +656,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$15:$F$15</c:f>
+              <c:f>Sprint!$C$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -596,7 +676,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -607,7 +687,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$B$14</c:f>
+              <c:f>Sprint!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -630,7 +710,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$13:$F$13</c:f>
+              <c:f>Sprint!$C$14:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -650,7 +730,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$14:$F$14</c:f>
+              <c:f>Sprint!$C$15:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -670,7 +750,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -684,7 +764,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="203184000"/>
         <c:axId val="203185536"/>
@@ -806,7 +885,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -838,14 +916,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -881,7 +959,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -920,7 +998,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -956,7 +1033,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$39:$F$39</c:f>
+              <c:f>Sprint!$C$39:$F$39</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -976,7 +1053,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$40:$F$40</c:f>
+              <c:f>Sprint!$C$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -996,7 +1073,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1022,7 +1099,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$39:$F$39</c:f>
+              <c:f>Sprint!$C$39:$F$39</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1042,7 +1119,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$41:$F$41</c:f>
+              <c:f>Sprint!$C$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1062,7 +1139,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1076,7 +1153,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="203224576"/>
         <c:axId val="203226112"/>
@@ -1198,7 +1274,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1230,14 +1305,379 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Burndown Chart Sprint 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Waktu perkiraan (baseline)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$60:$F$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8AFC-4EDF-A567-4D2A7E6BA605}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waktu sebenarnya</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$61:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8AFC-4EDF-A567-4D2A7E6BA605}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="203224576"/>
+        <c:axId val="203226112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="203224576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203226112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="203226112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203224576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1848,7 +2288,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1886,7 +2326,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4D9317-E42E-4604-AACF-4683186C73E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1901,6 +2341,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2198,18 +2676,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2225,15 +2703,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -2356,10 +2834,14 @@
         <v>35</v>
       </c>
       <c r="G8" s="2">
-        <v>4</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="2">
@@ -2378,10 +2860,14 @@
         <v>35</v>
       </c>
       <c r="G9" s="2">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="2">
@@ -2400,10 +2886,14 @@
         <v>35</v>
       </c>
       <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="5">
@@ -2422,10 +2912,14 @@
         <v>34</v>
       </c>
       <c r="G11" s="6">
-        <v>4</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="2">
@@ -2444,10 +2938,14 @@
         <v>34</v>
       </c>
       <c r="G12" s="6">
-        <v>4</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="5">
@@ -2466,10 +2964,14 @@
         <v>34</v>
       </c>
       <c r="G13" s="6">
-        <v>4</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="2">
@@ -2635,23 +3137,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2665,49 +3155,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="1:7">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -2722,52 +3192,55 @@
         <v>0</v>
       </c>
       <c r="G4" s="2">
+        <f>SUM(D4:F4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>2</v>
+        <f t="shared" ref="G5:G12" si="0">SUM(D5:F5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2782,52 +3255,55 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2842,82 +3318,105 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
         <v>2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="C13" s="4" t="s">
+    <row r="14" spans="1:7">
+      <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C3:C11)</f>
-        <v>12</v>
-      </c>
-      <c r="D14" s="2">
-        <f>C14-(SUM(D3:D11))</f>
-        <v>12</v>
-      </c>
-      <c r="E14" s="2">
-        <f>D14-(SUM(E3:E11))</f>
-        <v>6</v>
-      </c>
-      <c r="F14" s="2">
-        <f>E14-(SUM(F3:F11))</f>
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2">
+        <f>SUM(C4:C12)</f>
+        <v>12</v>
+      </c>
+      <c r="D15" s="2">
+        <f>C15-(SUM(D4:D12))</f>
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <f>D15-(SUM(E4:E12))</f>
+        <v>6</v>
+      </c>
+      <c r="F15" s="2">
+        <f>E15-(SUM(F4:F12))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2">
-        <f>SUM(C3:C11)</f>
+      <c r="C16" s="2">
+        <f>SUM(C4:C12)</f>
         <v>12</v>
       </c>
-      <c r="D15" s="2">
-        <f>C15-(C15/3)</f>
+      <c r="D16" s="2">
+        <f>C16-(C16/3)</f>
         <v>8</v>
       </c>
-      <c r="E15" s="2">
-        <f>D15-(C15/3)</f>
+      <c r="E16" s="2">
+        <f>D16-(C16/3)</f>
         <v>4</v>
       </c>
-      <c r="F15" s="2">
-        <f>E15-(C15/3)</f>
+      <c r="F16" s="2">
+        <f>E16-(C16/3)</f>
         <v>0</v>
       </c>
     </row>
@@ -2984,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ref="G27:G37" si="0">SUM(D27:F27)</f>
+        <f t="shared" ref="G27:G37" si="1">SUM(D27:F27)</f>
         <v>1</v>
       </c>
     </row>
@@ -3005,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3026,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3047,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3068,7 +3567,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3089,7 +3588,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3110,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3131,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3152,7 +3651,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3173,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3194,7 +3693,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3258,38 +3757,251 @@
       <c r="A46" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f>SUM(D49:F49)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2">
+        <f t="shared" ref="G50:G57" si="2">SUM(D50:F50)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="18"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="C59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="2">
+        <f>SUM(C49:C58)</f>
+        <v>6</v>
+      </c>
+      <c r="D60" s="2">
+        <f>C60-(SUM(D49:D58))</f>
+        <v>3</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="17"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2">
+        <f>SUM(C49:C58)</f>
+        <v>6</v>
+      </c>
+      <c r="D61" s="2">
+        <f>C61-(C61/3)</f>
+        <v>4</v>
+      </c>
+      <c r="E61" s="2">
+        <f>D61-(C61/3)</f>
+        <v>2</v>
+      </c>
+      <c r="F61" s="2">
+        <f>E61-(C61/3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" s="15" customFormat="1">
+      <c r="A69" s="14" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G26:G37 G4:G12 G49:G58" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C39" sqref="C38:C39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update logbook dan burndown chart Dec 27
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1463CB96-ED3E-4B9A-B2F5-5188463AA2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C605BA75-8AA7-403B-8D81-6A83A2443F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1441,6 +1441,9 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -2686,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3140,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3788,7 +3791,9 @@
       <c r="D49" s="2">
         <v>0.5</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2">
         <f>SUM(D49:F49)</f>
@@ -3805,7 +3810,9 @@
       <c r="D50" s="2">
         <v>0.5</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2">
+        <v>0</v>
+      </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2">
         <f t="shared" ref="G50:G57" si="2">SUM(D50:F50)</f>
@@ -3822,7 +3829,9 @@
       <c r="D51" s="2">
         <v>0</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2">
         <f t="shared" si="2"/>
@@ -3839,7 +3848,9 @@
       <c r="D52" s="2">
         <v>0.5</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2">
         <f t="shared" si="2"/>
@@ -3856,7 +3867,9 @@
       <c r="D53" s="2">
         <v>0.5</v>
       </c>
-      <c r="E53" s="2"/>
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2">
         <f t="shared" si="2"/>
@@ -3873,7 +3886,9 @@
       <c r="D54" s="2">
         <v>0</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2">
         <f t="shared" si="2"/>
@@ -3890,7 +3905,9 @@
       <c r="D55" s="2">
         <v>0.5</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2">
         <f t="shared" si="2"/>
@@ -3907,7 +3924,9 @@
       <c r="D56" s="2">
         <v>0.5</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2">
         <f t="shared" si="2"/>
@@ -3924,7 +3943,9 @@
       <c r="D57" s="2">
         <v>0</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2">
         <f t="shared" si="2"/>
@@ -3966,7 +3987,10 @@
         <f>C60-(SUM(D49:D58))</f>
         <v>3</v>
       </c>
-      <c r="E60" s="2"/>
+      <c r="E60" s="2">
+        <f>D60-(SUM(E49:E58))</f>
+        <v>3</v>
+      </c>
       <c r="F60" s="2"/>
       <c r="G60" s="17"/>
     </row>

</xml_diff>

<commit_message>
Update logbook dan burndown chart 28 Dec
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C605BA75-8AA7-403B-8D81-6A83A2443F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A8C2F7-3A60-47A8-8E4E-28BFFDDB0A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -118,12 +118,6 @@
     <t>memperlihatkan BUS Jenis PCI</t>
   </si>
   <si>
-    <t>penonton dapat memahami apa itu PCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">penonton dapat memhami apa itu ISA </t>
-  </si>
-  <si>
     <t xml:space="preserve">memperlihatkan BUS Jenis ISA </t>
   </si>
   <si>
@@ -139,15 +133,9 @@
     <t>memperlihatkan BUS Jenis MCA</t>
   </si>
   <si>
-    <t>penonton dapat memahami apa itu MCA</t>
-  </si>
-  <si>
     <t>memperlihatkan BUS Jenis FireWire</t>
   </si>
   <si>
-    <t>penonton dapat memahami apa itu FireWire</t>
-  </si>
-  <si>
     <t>memperlihatkan Elemen - elemen yang ada pada BUS</t>
   </si>
   <si>
@@ -214,12 +202,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>memperlihatkan animasi pada setiap perubahan slide dari BUS</t>
-  </si>
-  <si>
-    <t>penonton dapat lebih terkesan dengan slide yang dibawakan presenter</t>
-  </si>
-  <si>
     <t>Membuat kelemahan pada BUS</t>
   </si>
   <si>
@@ -265,9 +247,6 @@
     <t>Mempercantik slide arsitektur BUS</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
     <t>SPRINT 4</t>
   </si>
   <si>
@@ -296,13 +275,49 @@
   </si>
   <si>
     <t>Membuat pengertian tambahan dari Data Bus</t>
+  </si>
+  <si>
+    <t>memperlihatkan BUS Jenis USB</t>
+  </si>
+  <si>
+    <t>memperlihatkan BUS Jenis SCSI</t>
+  </si>
+  <si>
+    <t>memperlihatkan BUS Jenis Prosessor</t>
+  </si>
+  <si>
+    <t>memperlihatkan BUS Jenis AGP</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus AGP</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus MCA</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus FireWire</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus Prosessor</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus SCSI</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus PCI</t>
+  </si>
+  <si>
+    <t>penonton dapat memahami apa itu Bus USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penonton dapat memahami apa itu Bus ISA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,16 +389,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,13 +420,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -442,25 +444,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,13 +464,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -501,9 +487,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,10 +497,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1445,6 +1427,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2687,10 +2672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I20"/>
+  <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2706,15 +2691,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="B2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -2733,7 +2718,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
@@ -2755,8 +2740,8 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>35</v>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -2764,8 +2749,8 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>61</v>
+      <c r="I5" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -2781,8 +2766,8 @@
       <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>35</v>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G6" s="2">
         <v>4</v>
@@ -2790,8 +2775,8 @@
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>61</v>
+      <c r="I6" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -2807,8 +2792,8 @@
       <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>35</v>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G7" s="2">
         <v>4</v>
@@ -2816,8 +2801,8 @@
       <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>61</v>
+      <c r="I7" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -2833,8 +2818,8 @@
       <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>35</v>
+      <c r="F8" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
@@ -2842,8 +2827,8 @@
       <c r="H8" s="2">
         <v>2</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>61</v>
+      <c r="I8" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -2859,8 +2844,8 @@
       <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
+      <c r="F9" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
@@ -2868,8 +2853,8 @@
       <c r="H9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>61</v>
+      <c r="I9" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -2885,8 +2870,8 @@
       <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>35</v>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G10" s="2">
         <v>7</v>
@@ -2894,8 +2879,8 @@
       <c r="H10" s="2">
         <v>2</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>61</v>
+      <c r="I10" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -2905,23 +2890,23 @@
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>47</v>
+      <c r="D11" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="6">
+        <v>44</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="5">
         <v>2</v>
       </c>
       <c r="H11" s="2">
         <v>3</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>79</v>
+      <c r="I11" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -2931,23 +2916,23 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>52</v>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="6">
+        <v>45</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="5">
         <v>2</v>
       </c>
       <c r="H12" s="2">
         <v>3</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>79</v>
+      <c r="I12" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -2957,23 +2942,23 @@
       <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>51</v>
+      <c r="D13" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6">
+        <v>46</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="5">
         <v>2</v>
       </c>
       <c r="H13" s="2">
         <v>3</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>79</v>
+      <c r="I13" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -2984,16 +2969,16 @@
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3009,13 +2994,13 @@
         <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>34</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G15" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -3024,20 +3009,20 @@
       <c r="B16" s="2">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>34</v>
+      <c r="D16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G16" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3046,20 +3031,20 @@
       <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>34</v>
+      <c r="D17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G17" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3068,39 +3053,39 @@
       <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>41</v>
+      <c r="D18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G18" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>41</v>
+      <c r="D19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
@@ -3109,26 +3094,92 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="6">
+      <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="6">
-        <v>4</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="5">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="2">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="2">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="5">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3143,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
@@ -3153,9 +3204,9 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1">
-      <c r="A1" s="14" t="s">
-        <v>65</v>
+    <row r="1" spans="1:7" s="13" customFormat="1">
+      <c r="A1" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3180,7 +3231,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3201,7 +3252,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -3222,7 +3273,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -3243,7 +3294,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -3264,7 +3315,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -3285,7 +3336,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -3306,7 +3357,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -3327,7 +3378,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -3348,7 +3399,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -3423,9 +3474,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="15" customFormat="1">
-      <c r="A23" s="14" t="s">
-        <v>66</v>
+    <row r="23" spans="1:7" s="13" customFormat="1">
+      <c r="A23" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3450,7 +3501,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -3471,7 +3522,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -3492,7 +3543,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
@@ -3513,7 +3564,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -3534,7 +3585,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3555,7 +3606,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -3576,7 +3627,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="B32" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -3597,7 +3648,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -3618,7 +3669,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -3639,7 +3690,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -3660,7 +3711,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -3681,7 +3732,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -3756,9 +3807,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="15" customFormat="1">
-      <c r="A46" s="14" t="s">
-        <v>70</v>
+    <row r="46" spans="1:7" s="13" customFormat="1">
+      <c r="A46" s="12" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3783,7 +3834,7 @@
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C49" s="2">
         <v>0.5</v>
@@ -3794,7 +3845,9 @@
       <c r="E49" s="2">
         <v>0</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
       <c r="G49" s="2">
         <f>SUM(D49:F49)</f>
         <v>0.5</v>
@@ -3802,7 +3855,7 @@
     </row>
     <row r="50" spans="2:7">
       <c r="B50" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C50" s="2">
         <v>0.5</v>
@@ -3813,7 +3866,9 @@
       <c r="E50" s="2">
         <v>0</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
       <c r="G50" s="2">
         <f t="shared" ref="G50:G57" si="2">SUM(D50:F50)</f>
         <v>0.5</v>
@@ -3821,7 +3876,7 @@
     </row>
     <row r="51" spans="2:7">
       <c r="B51" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -3832,15 +3887,17 @@
       <c r="E51" s="2">
         <v>0</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="2">
+        <v>1</v>
+      </c>
       <c r="G51" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C52" s="2">
         <v>0.5</v>
@@ -3851,7 +3908,9 @@
       <c r="E52" s="2">
         <v>0</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
       <c r="G52" s="2">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -3859,7 +3918,7 @@
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C53" s="2">
         <v>0.5</v>
@@ -3870,7 +3929,9 @@
       <c r="E53" s="2">
         <v>0</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
       <c r="G53" s="2">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -3878,7 +3939,7 @@
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
@@ -3889,15 +3950,17 @@
       <c r="E54" s="2">
         <v>0</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
       <c r="G54" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2">
         <v>0.5</v>
@@ -3908,7 +3971,9 @@
       <c r="E55" s="2">
         <v>0</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2">
+        <v>0</v>
+      </c>
       <c r="G55" s="2">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -3916,7 +3981,7 @@
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C56" s="2">
         <v>0.5</v>
@@ -3927,7 +3992,9 @@
       <c r="E56" s="2">
         <v>0</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
       <c r="G56" s="2">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -3935,7 +4002,7 @@
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
@@ -3946,19 +4013,21 @@
       <c r="E57" s="2">
         <v>0</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
       <c r="G57" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="18"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
     </row>
     <row r="59" spans="2:7">
       <c r="C59" s="4" t="s">
@@ -3973,7 +4042,7 @@
       <c r="F59" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="17"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="4" t="s">
@@ -3991,8 +4060,11 @@
         <f>D60-(SUM(E49:E58))</f>
         <v>3</v>
       </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="17"/>
+      <c r="F60" s="2">
+        <f>E60-(SUM(F49:F58))</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="4" t="s">
@@ -4015,9 +4087,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" s="15" customFormat="1">
-      <c r="A69" s="14" t="s">
-        <v>80</v>
+    <row r="69" spans="1:1" s="13" customFormat="1">
+      <c r="A69" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update logbook dan burndown chart Dec 29
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A8C2F7-3A60-47A8-8E4E-28BFFDDB0A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53423DF1-658E-49BD-B33F-5918EAF0530B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -311,13 +311,43 @@
   </si>
   <si>
     <t xml:space="preserve">penonton dapat memahami apa itu Bus ISA </t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus ISA pada slide</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus PCI pada slide</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus USB pada slide</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Bus ISA</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Bus PCI</t>
+  </si>
+  <si>
+    <t>Membuat pengertian tambahan dari Bus USB</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus ISA didalamnya</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus PCI didalamnya</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus USB didalamnya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,8 +419,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +458,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -445,12 +488,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,13 +537,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1495,6 +1543,371 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8AFC-4EDF-A567-4D2A7E6BA605}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="203224576"/>
+        <c:axId val="203226112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="203224576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203226112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="203226112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203224576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Burndown Chart Sprint 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Waktu perkiraan (baseline)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$83:$F$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2593-4A48-80AB-BB20886B992C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waktu sebenarnya</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$84:$F$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2372,6 +2785,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2674,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2691,15 +3142,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -2980,8 +3431,12 @@
       <c r="G14" s="2">
         <v>3</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="H14" s="2">
+        <v>4</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="5">
@@ -3002,8 +3457,12 @@
       <c r="G15" s="2">
         <v>3</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="2">
+        <v>4</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="2">
@@ -3024,8 +3483,12 @@
       <c r="G16" s="2">
         <v>3</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="2">
+        <v>4</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="5">
@@ -3145,16 +3608,16 @@
         <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3167,16 +3630,16 @@
         <v>16</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G23" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3192,10 +3655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4087,9 +4550,242 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" s="13" customFormat="1">
+    <row r="69" spans="1:7" s="13" customFormat="1">
       <c r="A69" s="12" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="B72" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2">
+        <f>SUM(D72:F72)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="B73" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2">
+        <f t="shared" ref="G73:G80" si="3">SUM(D73:F73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="B75" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="B76" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="B78" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="B79" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="B80" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" s="15"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="C82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="2">
+        <f>SUM(C72:C81)</f>
+        <v>9</v>
+      </c>
+      <c r="D83" s="2">
+        <f>C83-(SUM(D72:D81))</f>
+        <v>6</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="14"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="2">
+        <f>SUM(C72:C81)</f>
+        <v>9</v>
+      </c>
+      <c r="D84" s="2">
+        <f>C84-(C84/3)</f>
+        <v>6</v>
+      </c>
+      <c r="E84" s="2">
+        <f>D84-(C84/3)</f>
+        <v>3</v>
+      </c>
+      <c r="F84" s="2">
+        <f>E84-(C84/3)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Penambahan isi Bus ISA beserta gambar Bus ISA // Update logbook dan burndown chart Dec 30
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\Tugas\TKPPL\Presentasi-Bus\Dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53423DF1-658E-49BD-B33F-5918EAF0530B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D71DC8-7BAC-4FCC-B4BB-6CFB546E36B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1843,6 +1843,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3125,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3434,8 +3437,8 @@
       <c r="H14" s="2">
         <v>4</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>95</v>
+      <c r="I14" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -3657,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4585,7 +4588,9 @@
       <c r="D72" s="2">
         <v>1</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2">
         <f>SUM(D72:F72)</f>
@@ -4602,11 +4607,13 @@
       <c r="D73" s="2">
         <v>0</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2">
         <f t="shared" ref="G73:G80" si="3">SUM(D73:F73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -4619,11 +4626,13 @@
       <c r="D74" s="2">
         <v>0</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -4636,7 +4645,9 @@
       <c r="D75" s="2">
         <v>1</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2">
+        <v>0</v>
+      </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2">
         <f t="shared" si="3"/>
@@ -4653,11 +4664,13 @@
       <c r="D76" s="2">
         <v>0</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="2">
+        <v>1</v>
+      </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -4670,7 +4683,9 @@
       <c r="D77" s="2">
         <v>0</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2">
         <f t="shared" si="3"/>
@@ -4687,7 +4702,9 @@
       <c r="D78" s="2">
         <v>1</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="2">
+        <v>0</v>
+      </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2">
         <f t="shared" si="3"/>
@@ -4704,11 +4721,13 @@
       <c r="D79" s="2">
         <v>0</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="2">
+        <v>1</v>
+      </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4721,7 +4740,9 @@
       <c r="D80" s="2">
         <v>0</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="2">
+        <v>0</v>
+      </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2">
         <f t="shared" si="3"/>
@@ -4763,7 +4784,10 @@
         <f>C83-(SUM(D72:D81))</f>
         <v>6</v>
       </c>
-      <c r="E83" s="2"/>
+      <c r="E83" s="2">
+        <f>D83-(SUM(E72:E81))</f>
+        <v>2</v>
+      </c>
       <c r="F83" s="2"/>
       <c r="G83" s="14"/>
     </row>

</xml_diff>

<commit_message>
Update Logbook and Burndown Chart 31 Dec
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\Tugas\TKPPL\Presentasi-Bus\Dokumen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D71DC8-7BAC-4FCC-B4BB-6CFB546E36B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BF8991-DD89-46E8-AB2F-B4ED32FE250C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t xml:space="preserve">penonton dapat memahami apa itu Bus ISA </t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Mendesign dan menuliskan pengertian Bus ISA pada slide</t>
@@ -347,7 +344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,16 +416,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,11 +447,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -488,13 +472,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,17 +520,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1846,6 +1825,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3128,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3145,15 +3127,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -3463,8 +3445,8 @@
       <c r="H15" s="2">
         <v>4</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>95</v>
+      <c r="I15" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -3489,8 +3471,8 @@
       <c r="H16" s="2">
         <v>4</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>95</v>
+      <c r="I16" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:9">
@@ -3660,8 +3642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4580,7 +4562,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="B72" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -4591,7 +4573,9 @@
       <c r="E72" s="2">
         <v>0</v>
       </c>
-      <c r="F72" s="2"/>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
       <c r="G72" s="2">
         <f>SUM(D72:F72)</f>
         <v>1</v>
@@ -4599,7 +4583,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
@@ -4610,7 +4594,9 @@
       <c r="E73" s="2">
         <v>1</v>
       </c>
-      <c r="F73" s="2"/>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
       <c r="G73" s="2">
         <f t="shared" ref="G73:G80" si="3">SUM(D73:F73)</f>
         <v>1</v>
@@ -4618,7 +4604,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="B74" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -4629,7 +4615,9 @@
       <c r="E74" s="2">
         <v>1</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
       <c r="G74" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -4637,7 +4625,7 @@
     </row>
     <row r="75" spans="1:7">
       <c r="B75" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -4648,7 +4636,9 @@
       <c r="E75" s="2">
         <v>0</v>
       </c>
-      <c r="F75" s="2"/>
+      <c r="F75" s="2">
+        <v>0</v>
+      </c>
       <c r="G75" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -4656,7 +4646,7 @@
     </row>
     <row r="76" spans="1:7">
       <c r="B76" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2">
         <v>1</v>
@@ -4667,7 +4657,9 @@
       <c r="E76" s="2">
         <v>1</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2">
+        <v>0</v>
+      </c>
       <c r="G76" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -4675,7 +4667,7 @@
     </row>
     <row r="77" spans="1:7">
       <c r="B77" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -4686,15 +4678,17 @@
       <c r="E77" s="2">
         <v>0</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2">
+        <v>1</v>
+      </c>
       <c r="G77" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -4705,7 +4699,9 @@
       <c r="E78" s="2">
         <v>0</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2">
+        <v>0</v>
+      </c>
       <c r="G78" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -4713,7 +4709,7 @@
     </row>
     <row r="79" spans="1:7">
       <c r="B79" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -4724,7 +4720,9 @@
       <c r="E79" s="2">
         <v>1</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
       <c r="G79" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -4732,7 +4730,7 @@
     </row>
     <row r="80" spans="1:7">
       <c r="B80" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C80" s="2">
         <v>1</v>
@@ -4743,10 +4741,12 @@
       <c r="E80" s="2">
         <v>0</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2">
+        <v>1</v>
+      </c>
       <c r="G80" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:7">
@@ -4788,7 +4788,10 @@
         <f>D83-(SUM(E72:E81))</f>
         <v>2</v>
       </c>
-      <c r="F83" s="2"/>
+      <c r="F83" s="2">
+        <f>E83-(SUM(F72:F81))</f>
+        <v>0</v>
+      </c>
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="2:7">

</xml_diff>

<commit_message>
mengupdate Logbook dan menambahkan slide pengertian AGP
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BF8991-DD89-46E8-AB2F-B4ED32FE250C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -338,12 +332,33 @@
   </si>
   <si>
     <t>Membuat slide baru dengan menambahkan gambar Bus USB didalamnya</t>
+  </si>
+  <si>
+    <t>SPRINT 5</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus SCSI didalamnya</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus Prosessor didalamnya</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus AGP didalamnya</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus SCSI pada slide</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus Prosessor pada slide</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus AGP pada slide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -543,7 +558,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -582,6 +597,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -590,26 +606,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -685,7 +681,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -759,7 +755,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -773,12 +769,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203184000"/>
-        <c:axId val="203185536"/>
+        <c:axId val="196752512"/>
+        <c:axId val="196754048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203184000"/>
+        <c:axId val="196752512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203185536"/>
+        <c:crossAx val="196754048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -829,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203185536"/>
+        <c:axId val="196754048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203184000"/>
+        <c:crossAx val="196752512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -894,6 +891,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -925,14 +923,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -968,7 +966,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1007,6 +1005,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1082,7 +1081,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1148,7 +1147,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1162,12 +1161,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203224576"/>
-        <c:axId val="203226112"/>
+        <c:axId val="196793088"/>
+        <c:axId val="196794624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203224576"/>
+        <c:axId val="196793088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203226112"/>
+        <c:crossAx val="196794624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1218,7 +1218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203226112"/>
+        <c:axId val="196794624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,7 +1269,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203224576"/>
+        <c:crossAx val="196793088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1283,6 +1283,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1314,14 +1315,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1357,7 +1358,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1396,6 +1397,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1462,7 +1464,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8AFC-4EDF-A567-4D2A7E6BA605}"/>
             </c:ext>
@@ -1519,7 +1521,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8AFC-4EDF-A567-4D2A7E6BA605}"/>
             </c:ext>
@@ -1533,12 +1535,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203224576"/>
-        <c:axId val="203226112"/>
+        <c:axId val="196637056"/>
+        <c:axId val="196638592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203224576"/>
+        <c:axId val="196637056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,7 +1584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203226112"/>
+        <c:crossAx val="196638592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1589,7 +1592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203226112"/>
+        <c:axId val="196638592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203224576"/>
+        <c:crossAx val="196637056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1654,6 +1657,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1685,14 +1689,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1728,7 +1732,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1767,6 +1771,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1833,7 +1838,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -1890,7 +1895,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -1904,12 +1909,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203224576"/>
-        <c:axId val="203226112"/>
+        <c:axId val="196670976"/>
+        <c:axId val="196672512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203224576"/>
+        <c:axId val="196670976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203226112"/>
+        <c:crossAx val="196672512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1960,7 +1966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203226112"/>
+        <c:axId val="196672512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,7 +2017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203224576"/>
+        <c:crossAx val="196670976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2025,6 +2031,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2056,14 +2063,388 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Burndown Chart Sprint 5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Waktu Perkiraan (Baseline)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$103:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2593-4A48-80AB-BB20886B992C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waktu sebenarnya</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$104:$F$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2593-4A48-80AB-BB20886B992C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="127586304"/>
+        <c:axId val="127587840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="127586304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="127587840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="127587840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="127586304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2674,7 +3055,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2712,7 +3093,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2750,7 +3131,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2788,7 +3169,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2803,6 +3184,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3100,14 +3519,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3639,11 +4058,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="U96" sqref="U96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4749,7 +5168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="1:7">
       <c r="B81" s="15"/>
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
@@ -4757,7 +5176,7 @@
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="1:7">
       <c r="C82" s="4" t="s">
         <v>15</v>
       </c>
@@ -4772,7 +5191,7 @@
       </c>
       <c r="G82" s="14"/>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="1:7">
       <c r="B83" s="4" t="s">
         <v>7</v>
       </c>
@@ -4794,7 +5213,7 @@
       </c>
       <c r="G83" s="14"/>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="1:7">
       <c r="B84" s="4" t="s">
         <v>10</v>
       </c>
@@ -4812,6 +5231,223 @@
       </c>
       <c r="F84" s="2">
         <f>E84-(C84/3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="13" customFormat="1">
+      <c r="A92" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="B94" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="B95" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0</v>
+      </c>
+      <c r="G95" s="2">
+        <f>SUM(D95:F95)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="B96" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C96" s="2">
+        <v>1</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0</v>
+      </c>
+      <c r="G96" s="2">
+        <f t="shared" ref="G96:G100" si="4">SUM(D96:F96)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C97" s="2">
+        <v>1</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0</v>
+      </c>
+      <c r="G97" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="2">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0</v>
+      </c>
+      <c r="G98" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" s="2">
+        <v>1</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0</v>
+      </c>
+      <c r="G99" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100" s="2">
+        <v>1</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0</v>
+      </c>
+      <c r="G100" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101" s="15"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="C102" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" s="14"/>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="2">
+        <f>SUM(C95:C101)</f>
+        <v>6</v>
+      </c>
+      <c r="D103" s="2">
+        <f>C103-(SUM(D95:D101))</f>
+        <v>3</v>
+      </c>
+      <c r="E103" s="2">
+        <f>D103-(SUM(E95:E101))</f>
+        <v>3</v>
+      </c>
+      <c r="F103" s="2">
+        <f>E103-(SUM(F95:F101))</f>
+        <v>3</v>
+      </c>
+      <c r="G103" s="14"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="2">
+        <f>SUM(C95:C101)</f>
+        <v>6</v>
+      </c>
+      <c r="D104" s="2">
+        <f>C104-(C104/3)</f>
+        <v>4</v>
+      </c>
+      <c r="E104" s="2">
+        <f>D104-(C104/3)</f>
+        <v>2</v>
+      </c>
+      <c r="F104" s="2">
+        <f>E104-(C104/3)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
menambahkan slide gambar BUS AGP
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -597,7 +597,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -771,11 +770,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196752512"/>
-        <c:axId val="196754048"/>
+        <c:axId val="194528384"/>
+        <c:axId val="194529920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196752512"/>
+        <c:axId val="194528384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196754048"/>
+        <c:crossAx val="194529920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196754048"/>
+        <c:axId val="194529920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,7 +876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196752512"/>
+        <c:crossAx val="194528384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -891,7 +890,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1163,11 +1161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196793088"/>
-        <c:axId val="196794624"/>
+        <c:axId val="194568960"/>
+        <c:axId val="194570496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196793088"/>
+        <c:axId val="194568960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196794624"/>
+        <c:crossAx val="194570496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1218,7 +1216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196794624"/>
+        <c:axId val="194570496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,7 +1267,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196793088"/>
+        <c:crossAx val="194568960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1537,11 +1535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196637056"/>
-        <c:axId val="196638592"/>
+        <c:axId val="194408832"/>
+        <c:axId val="194410368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196637056"/>
+        <c:axId val="194408832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196638592"/>
+        <c:crossAx val="194410368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196638592"/>
+        <c:axId val="194410368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196637056"/>
+        <c:crossAx val="194408832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1911,11 +1909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196670976"/>
-        <c:axId val="196672512"/>
+        <c:axId val="194577920"/>
+        <c:axId val="194579456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196670976"/>
+        <c:axId val="194577920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196672512"/>
+        <c:crossAx val="194579456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1966,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196672512"/>
+        <c:axId val="194579456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2017,7 +2015,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196670976"/>
+        <c:crossAx val="194577920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2203,10 +2201,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2285,11 +2283,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127586304"/>
-        <c:axId val="127587840"/>
+        <c:axId val="194635264"/>
+        <c:axId val="194636800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127586304"/>
+        <c:axId val="194635264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127587840"/>
+        <c:crossAx val="194636800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2340,7 +2338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127587840"/>
+        <c:axId val="194636800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,7 +2389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127586304"/>
+        <c:crossAx val="194635264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3055,7 +3053,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3093,7 +3091,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3131,7 +3129,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3169,7 +3167,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3207,7 +3205,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3519,7 +3517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4061,8 +4059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="U96" sqref="U96"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5291,14 +5289,14 @@
         <v>0</v>
       </c>
       <c r="E96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="2">
         <v>0</v>
       </c>
       <c r="G96" s="2">
         <f t="shared" ref="G96:G100" si="4">SUM(D96:F96)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="2:7">
@@ -5333,14 +5331,14 @@
         <v>0</v>
       </c>
       <c r="E98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="2">
         <v>0</v>
       </c>
       <c r="G98" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:7">
@@ -5375,14 +5373,14 @@
         <v>0</v>
       </c>
       <c r="E100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="2">
         <v>0</v>
       </c>
       <c r="G100" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="2:7">
@@ -5422,11 +5420,11 @@
       </c>
       <c r="E103" s="2">
         <f>D103-(SUM(E95:E101))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F103" s="2">
         <f>E103-(SUM(F95:F101))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G103" s="14"/>
     </row>

</xml_diff>

<commit_message>
Update logbook dan burndown chart Jan 4
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407C4F7-A530-4023-9D1D-01DBFCC15781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -353,13 +359,52 @@
   </si>
   <si>
     <t>Mendesign dan menuliskan pengertian Bus AGP pada slide</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>SPRINT 6</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan kata terima kasih pada slide</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan keuntungan dan kerugian masing - masing elemen jenis bus</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan elemen bus berdasarkan metode arbitrasi</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan elemen bus berdasarkan jenisnya</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan elemen bus berdasarkan timing</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan elemen bus berdasarkan lebar bus</t>
+  </si>
+  <si>
+    <t>Menambahkan slide baru dengan menambahkan elemen bus berdasarkan jenis transfer data</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus Firewire pada slide</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus Firewire didalamnya</t>
+  </si>
+  <si>
+    <t>Mendesign dan menuliskan pengertian Bus MCA pada slide</t>
+  </si>
+  <si>
+    <t>Membuat slide baru dengan menambahkan gambar Bus MCA didalamnya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,8 +476,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +515,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -487,12 +545,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,13 +594,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -558,7 +621,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -605,6 +668,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -680,7 +763,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -754,7 +837,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -768,7 +851,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="194528384"/>
         <c:axId val="194529920"/>
@@ -921,14 +1003,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -964,7 +1046,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1003,7 +1085,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1079,7 +1160,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1145,7 +1226,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F56-4258-A1B1-9890DA84A2ED}"/>
             </c:ext>
@@ -1159,7 +1240,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="194568960"/>
         <c:axId val="194570496"/>
@@ -1281,7 +1361,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1313,14 +1392,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1356,7 +1435,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1395,7 +1474,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1462,7 +1540,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8AFC-4EDF-A567-4D2A7E6BA605}"/>
             </c:ext>
@@ -1519,7 +1597,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8AFC-4EDF-A567-4D2A7E6BA605}"/>
             </c:ext>
@@ -1533,7 +1611,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="194408832"/>
         <c:axId val="194410368"/>
@@ -1655,7 +1732,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1687,14 +1763,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1730,7 +1806,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1769,7 +1845,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1836,7 +1911,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -1893,7 +1968,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -1907,7 +1982,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="194577920"/>
         <c:axId val="194579456"/>
@@ -2029,7 +2103,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2061,14 +2134,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2104,7 +2177,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2143,7 +2216,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2210,7 +2282,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -2267,7 +2339,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2593-4A48-80AB-BB20886B992C}"/>
             </c:ext>
@@ -2281,7 +2353,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="194635264"/>
         <c:axId val="194636800"/>
@@ -2403,7 +2474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2435,14 +2505,379 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Burndown Chart Sprint 5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Waktu Perkiraan (Baseline)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$128:$F$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B96A-4189-AC50-56D0D941E018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waktu sebenarnya</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$C$39:$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hari 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hari 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hari 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hari 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$C$129:$F$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B96A-4189-AC50-56D0D941E018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="194635264"/>
+        <c:axId val="194636800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="194635264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="194636800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="194636800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="194635264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3053,7 +3488,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,7 +3526,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,7 +3564,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6A3912-2478-4A53-ABBA-97AFAB7A15BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3167,7 +3602,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3205,7 +3640,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7AA64-B5B4-441A-99C7-79DFE3521514}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3220,6 +3655,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FD90BF1-DAB0-4CB6-A4F8-2C865B3C7E14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3517,18 +3990,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3544,15 +4017,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -3909,10 +4382,14 @@
         <v>32</v>
       </c>
       <c r="G17" s="2">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="2">
@@ -3931,10 +4408,14 @@
         <v>32</v>
       </c>
       <c r="G18" s="2">
-        <v>3</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="5">
@@ -3953,10 +4434,14 @@
         <v>32</v>
       </c>
       <c r="G19" s="2">
-        <v>3</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="2">
@@ -3975,10 +4460,14 @@
         <v>32</v>
       </c>
       <c r="G20" s="2">
-        <v>3</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>6</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="5">
@@ -3997,10 +4486,14 @@
         <v>32</v>
       </c>
       <c r="G21" s="2">
-        <v>3</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>6</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="2">
@@ -4021,8 +4514,12 @@
       <c r="G22" s="2">
         <v>1</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="H22" s="2">
+        <v>6</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="5">
@@ -4041,10 +4538,14 @@
         <v>37</v>
       </c>
       <c r="G23" s="2">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="H23" s="2">
+        <v>6</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4056,16 +4557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="H136" sqref="H136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="74.5703125" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5299,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="1:7">
       <c r="B97" s="3" t="s">
         <v>109</v>
       </c>
@@ -5320,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:7">
+    <row r="98" spans="1:7">
       <c r="B98" s="3" t="s">
         <v>106</v>
       </c>
@@ -5341,7 +5842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:7">
+    <row r="99" spans="1:7">
       <c r="B99" s="3" t="s">
         <v>110</v>
       </c>
@@ -5362,7 +5863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:7">
+    <row r="100" spans="1:7">
       <c r="B100" s="3" t="s">
         <v>107</v>
       </c>
@@ -5383,7 +5884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:7">
+    <row r="101" spans="1:7">
       <c r="B101" s="15"/>
       <c r="C101" s="14"/>
       <c r="D101" s="14"/>
@@ -5391,7 +5892,7 @@
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
     </row>
-    <row r="102" spans="2:7">
+    <row r="102" spans="1:7">
       <c r="C102" s="4" t="s">
         <v>15</v>
       </c>
@@ -5406,7 +5907,7 @@
       </c>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="2:7">
+    <row r="103" spans="1:7">
       <c r="B103" s="4" t="s">
         <v>7</v>
       </c>
@@ -5428,7 +5929,7 @@
       </c>
       <c r="G103" s="14"/>
     </row>
-    <row r="104" spans="2:7">
+    <row r="104" spans="1:7">
       <c r="B104" s="4" t="s">
         <v>10</v>
       </c>
@@ -5446,6 +5947,268 @@
       </c>
       <c r="F104" s="2">
         <f>E104-(C104/3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="13" customFormat="1">
+      <c r="A112" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7">
+      <c r="B114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C115" s="2">
+        <v>1</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2">
+        <f>SUM(D115:F115)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="B116" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C116" s="2">
+        <v>1</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2">
+        <f t="shared" ref="G116:G125" si="5">SUM(D116:F116)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" s="2">
+        <v>1</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C118" s="2">
+        <v>1</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C119" s="2">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="2">
+        <v>1</v>
+      </c>
+      <c r="D120" s="2">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="B121" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C121" s="5">
+        <v>2</v>
+      </c>
+      <c r="D121" s="5">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="B122" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C122" s="5">
+        <v>1</v>
+      </c>
+      <c r="D122" s="5">
+        <v>0</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="B123" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C123" s="5">
+        <v>1</v>
+      </c>
+      <c r="D123" s="5">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7">
+      <c r="B124" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C124" s="5">
+        <v>1</v>
+      </c>
+      <c r="D124" s="5">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125" s="5">
+        <v>1</v>
+      </c>
+      <c r="D125" s="5">
+        <v>0</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7">
+      <c r="C127" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7">
+      <c r="B128" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" s="2">
+        <f>SUM(C115:C125)</f>
+        <v>12</v>
+      </c>
+      <c r="D128" s="2">
+        <f>C128-(SUM(D115:D125))</f>
+        <v>7</v>
+      </c>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+    </row>
+    <row r="129" spans="2:6">
+      <c r="B129" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" s="2">
+        <f>SUM(C115:C125)</f>
+        <v>12</v>
+      </c>
+      <c r="D129" s="2">
+        <f>C129-(C129/3)</f>
+        <v>8</v>
+      </c>
+      <c r="E129" s="2">
+        <f>D129-(C129/3)</f>
+        <v>4</v>
+      </c>
+      <c r="F129" s="2">
+        <f>E129-(C129/3)</f>
         <v>0</v>
       </c>
     </row>
@@ -5453,7 +6216,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G26:G37 G4:G12 G49:G58" formulaRange="1"/>
+    <ignoredError sqref="G26:G37 G4:G12 G49:G58 G115:G125 G72:G80 G95:G100" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Update logbook dan burndown chart Jan 5
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407C4F7-A530-4023-9D1D-01DBFCC15781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0A4A0B-9DA8-4B29-8DE7-4AA7255EEE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -2642,6 +2642,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4000,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4560,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5985,7 +5988,9 @@
       <c r="D115" s="2">
         <v>1</v>
       </c>
-      <c r="E115" s="2"/>
+      <c r="E115" s="2">
+        <v>0</v>
+      </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2">
         <f>SUM(D115:F115)</f>
@@ -6002,11 +6007,13 @@
       <c r="D116" s="2">
         <v>0</v>
       </c>
-      <c r="E116" s="2"/>
+      <c r="E116" s="2">
+        <v>1</v>
+      </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2">
         <f t="shared" ref="G116:G125" si="5">SUM(D116:F116)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="2:7">
@@ -6019,7 +6026,9 @@
       <c r="D117" s="2">
         <v>1</v>
       </c>
-      <c r="E117" s="2"/>
+      <c r="E117" s="2">
+        <v>0</v>
+      </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2">
         <f t="shared" si="5"/>
@@ -6036,11 +6045,13 @@
       <c r="D118" s="2">
         <v>0</v>
       </c>
-      <c r="E118" s="2"/>
+      <c r="E118" s="2">
+        <v>1</v>
+      </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="2:7">
@@ -6053,7 +6064,9 @@
       <c r="D119" s="2">
         <v>1</v>
       </c>
-      <c r="E119" s="2"/>
+      <c r="E119" s="2">
+        <v>0</v>
+      </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2">
         <f t="shared" si="5"/>
@@ -6070,7 +6083,9 @@
       <c r="D120" s="2">
         <v>1</v>
       </c>
-      <c r="E120" s="2"/>
+      <c r="E120" s="2">
+        <v>0</v>
+      </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2">
         <f t="shared" si="5"/>
@@ -6087,11 +6102,13 @@
       <c r="D121" s="5">
         <v>1</v>
       </c>
-      <c r="E121" s="2"/>
+      <c r="E121" s="2">
+        <v>1</v>
+      </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="2:7">
@@ -6104,11 +6121,13 @@
       <c r="D122" s="5">
         <v>0</v>
       </c>
-      <c r="E122" s="2"/>
+      <c r="E122" s="2">
+        <v>1</v>
+      </c>
       <c r="F122" s="2"/>
       <c r="G122" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="2:7">
@@ -6121,7 +6140,9 @@
       <c r="D123" s="5">
         <v>0</v>
       </c>
-      <c r="E123" s="2"/>
+      <c r="E123" s="2">
+        <v>0</v>
+      </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2">
         <f t="shared" si="5"/>
@@ -6138,7 +6159,9 @@
       <c r="D124" s="5">
         <v>0</v>
       </c>
-      <c r="E124" s="2"/>
+      <c r="E124" s="2">
+        <v>0</v>
+      </c>
       <c r="F124" s="2"/>
       <c r="G124" s="2">
         <f t="shared" si="5"/>
@@ -6155,7 +6178,9 @@
       <c r="D125" s="5">
         <v>0</v>
       </c>
-      <c r="E125" s="2"/>
+      <c r="E125" s="2">
+        <v>0</v>
+      </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2">
         <f t="shared" si="5"/>
@@ -6188,7 +6213,10 @@
         <f>C128-(SUM(D115:D125))</f>
         <v>7</v>
       </c>
-      <c r="E128" s="2"/>
+      <c r="E128" s="2">
+        <f>D128-(SUM(E115:E125))</f>
+        <v>3</v>
+      </c>
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="2:6">

</xml_diff>

<commit_message>
Update logbook dan burndown chart Jan 6
</commit_message>
<xml_diff>
--- a/Dokumen/Product Backlog & Burndown Chart.xlsx
+++ b/Dokumen/Product Backlog & Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0A4A0B-9DA8-4B29-8DE7-4AA7255EEE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEBBC67-9194-4E14-8504-8D573C458884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -359,9 +359,6 @@
   </si>
   <si>
     <t>Mendesign dan menuliskan pengertian Bus AGP pada slide</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>SPRINT 6</t>
@@ -404,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,16 +473,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,11 +504,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -545,13 +529,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,17 +577,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2645,6 +2624,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4003,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4020,15 +4002,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="15.75">
       <c r="B4" s="1" t="s">
@@ -4468,8 +4450,8 @@
       <c r="H20" s="2">
         <v>6</v>
       </c>
-      <c r="I20" s="16" t="s">
-        <v>111</v>
+      <c r="I20" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -4494,8 +4476,8 @@
       <c r="H21" s="2">
         <v>6</v>
       </c>
-      <c r="I21" s="16" t="s">
-        <v>111</v>
+      <c r="I21" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -4520,8 +4502,8 @@
       <c r="H22" s="2">
         <v>6</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>111</v>
+      <c r="I22" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -4546,8 +4528,8 @@
       <c r="H23" s="2">
         <v>6</v>
       </c>
-      <c r="I23" s="16" t="s">
-        <v>111</v>
+      <c r="I23" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4563,8 +4545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5955,7 +5937,7 @@
     </row>
     <row r="112" spans="1:7" s="13" customFormat="1">
       <c r="A112" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="2:7">
@@ -5980,7 +5962,7 @@
     </row>
     <row r="115" spans="2:7">
       <c r="B115" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C115" s="2">
         <v>1</v>
@@ -5991,7 +5973,9 @@
       <c r="E115" s="2">
         <v>0</v>
       </c>
-      <c r="F115" s="2"/>
+      <c r="F115" s="2">
+        <v>0</v>
+      </c>
       <c r="G115" s="2">
         <f>SUM(D115:F115)</f>
         <v>1</v>
@@ -5999,7 +5983,7 @@
     </row>
     <row r="116" spans="2:7">
       <c r="B116" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C116" s="2">
         <v>1</v>
@@ -6010,7 +5994,9 @@
       <c r="E116" s="2">
         <v>1</v>
       </c>
-      <c r="F116" s="2"/>
+      <c r="F116" s="2">
+        <v>0</v>
+      </c>
       <c r="G116" s="2">
         <f t="shared" ref="G116:G125" si="5">SUM(D116:F116)</f>
         <v>1</v>
@@ -6018,7 +6004,7 @@
     </row>
     <row r="117" spans="2:7">
       <c r="B117" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C117" s="2">
         <v>1</v>
@@ -6029,7 +6015,9 @@
       <c r="E117" s="2">
         <v>0</v>
       </c>
-      <c r="F117" s="2"/>
+      <c r="F117" s="2">
+        <v>0</v>
+      </c>
       <c r="G117" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -6037,7 +6025,7 @@
     </row>
     <row r="118" spans="2:7">
       <c r="B118" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C118" s="2">
         <v>1</v>
@@ -6048,7 +6036,9 @@
       <c r="E118" s="2">
         <v>1</v>
       </c>
-      <c r="F118" s="2"/>
+      <c r="F118" s="2">
+        <v>0</v>
+      </c>
       <c r="G118" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -6056,7 +6046,7 @@
     </row>
     <row r="119" spans="2:7">
       <c r="B119" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119" s="2">
         <v>1</v>
@@ -6067,7 +6057,9 @@
       <c r="E119" s="2">
         <v>0</v>
       </c>
-      <c r="F119" s="2"/>
+      <c r="F119" s="2">
+        <v>0</v>
+      </c>
       <c r="G119" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -6075,7 +6067,7 @@
     </row>
     <row r="120" spans="2:7">
       <c r="B120" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C120" s="2">
         <v>1</v>
@@ -6086,7 +6078,9 @@
       <c r="E120" s="2">
         <v>0</v>
       </c>
-      <c r="F120" s="2"/>
+      <c r="F120" s="2">
+        <v>0</v>
+      </c>
       <c r="G120" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -6094,7 +6088,7 @@
     </row>
     <row r="121" spans="2:7">
       <c r="B121" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C121" s="5">
         <v>2</v>
@@ -6105,7 +6099,9 @@
       <c r="E121" s="2">
         <v>1</v>
       </c>
-      <c r="F121" s="2"/>
+      <c r="F121" s="2">
+        <v>0</v>
+      </c>
       <c r="G121" s="2">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -6113,7 +6109,7 @@
     </row>
     <row r="122" spans="2:7">
       <c r="B122" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C122" s="5">
         <v>1</v>
@@ -6124,7 +6120,9 @@
       <c r="E122" s="2">
         <v>1</v>
       </c>
-      <c r="F122" s="2"/>
+      <c r="F122" s="2">
+        <v>0</v>
+      </c>
       <c r="G122" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -6132,7 +6130,7 @@
     </row>
     <row r="123" spans="2:7">
       <c r="B123" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C123" s="5">
         <v>1</v>
@@ -6143,15 +6141,17 @@
       <c r="E123" s="2">
         <v>0</v>
       </c>
-      <c r="F123" s="2"/>
+      <c r="F123" s="2">
+        <v>1</v>
+      </c>
       <c r="G123" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="2:7">
       <c r="B124" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C124" s="5">
         <v>1</v>
@@ -6162,15 +6162,17 @@
       <c r="E124" s="2">
         <v>0</v>
       </c>
-      <c r="F124" s="2"/>
+      <c r="F124" s="2">
+        <v>1</v>
+      </c>
       <c r="G124" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:7">
       <c r="B125" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C125" s="5">
         <v>1</v>
@@ -6181,10 +6183,12 @@
       <c r="E125" s="2">
         <v>0</v>
       </c>
-      <c r="F125" s="2"/>
+      <c r="F125" s="2">
+        <v>1</v>
+      </c>
       <c r="G125" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="2:7">
@@ -6217,7 +6221,10 @@
         <f>D128-(SUM(E115:E125))</f>
         <v>3</v>
       </c>
-      <c r="F128" s="2"/>
+      <c r="F128" s="2">
+        <f>E128-(SUM(F115:F125))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="2:6">
       <c r="B129" s="4" t="s">

</xml_diff>